<commit_message>
TST: mitutoyo uniform and nonuniform tests
</commit_message>
<xml_diff>
--- a/test/file_format_examples/mitutoyo_mock.xlsx
+++ b/test/file_format_examples/mitutoyo_mock.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12525"/>
+    <workbookView windowWidth="28800" windowHeight="12930"/>
   </bookViews>
   <sheets>
     <sheet name="Certificate" sheetId="1" r:id="rId1"/>
@@ -15,9 +15,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>10- Oct -2022</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>Work Name</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>Oprator</t>
+  </si>
+  <si>
+    <t>Mitutoyo</t>
+  </si>
+  <si>
+    <t>Measuring Tool</t>
+  </si>
+  <si>
+    <t>SurfTest</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Ver2.00</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>ISO 1997</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Profile</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Cut-Off</t>
+  </si>
+  <si>
+    <t>0.08mm</t>
+  </si>
+  <si>
+    <t>λs</t>
+  </si>
+  <si>
+    <t>2.5µm</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>GAUSS</t>
   </si>
   <si>
     <t xml:space="preserve">Ra     0.018  µm      </t>
@@ -41,9 +104,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -64,9 +127,16 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -80,9 +150,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -111,18 +187,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -135,7 +212,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -149,14 +256,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -164,45 +263,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -217,7 +280,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -229,13 +298,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -247,7 +316,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -259,145 +454,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,6 +471,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -431,32 +509,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -472,15 +529,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -503,8 +551,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -513,148 +576,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -670,6 +733,9 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -990,17 +1056,92 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="E2"/>
+  <dimension ref="B2:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <sheetData>
     <row r="2" spans="5:5">
       <c r="E2" s="3" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="5:5">
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="B43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5">
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5">
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5">
+      <c r="B49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1015,7 +1156,7 @@
   <dimension ref="A1:F31517"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1027,7 +1168,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1">
         <v>0.0005</v>
@@ -1038,7 +1179,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1">
         <v>0.001</v>
@@ -1049,7 +1190,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1">
         <v>0.0015</v>
@@ -1060,7 +1201,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="E4" s="1">
         <v>0.002</v>
@@ -1071,7 +1212,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1">
         <v>0.0025</v>

</xml_diff>

<commit_message>
MAINT: removed relic from mitutoyo mock excel files
</commit_message>
<xml_diff>
--- a/test/file_format_examples/mitutoyo_mock.xlsx
+++ b/test/file_format_examples/mitutoyo_mock.xlsx
@@ -15,12 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>10- Oct -2022</t>
-  </si>
-  <si>
-    <t>and</t>
   </si>
   <si>
     <t>Work Name</t>
@@ -103,10 +100,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -127,16 +124,23 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -150,21 +154,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -180,10 +169,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -203,46 +193,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,7 +209,52 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -280,7 +277,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,31 +325,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,31 +349,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,7 +373,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -388,7 +403,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -401,66 +458,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -500,17 +497,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -529,6 +515,32 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -556,162 +568,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1058,8 +1055,8 @@
   <sheetPr/>
   <dimension ref="B2:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1069,79 +1066,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="5:5">
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-    </row>
     <row r="43" spans="2:5">
       <c r="B43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
         <v>2</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>3</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>4</v>
-      </c>
-      <c r="E43" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="44" spans="2:5">
       <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
         <v>6</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>7</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="47" spans="2:5">
       <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" t="s">
         <v>10</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>11</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>12</v>
-      </c>
-      <c r="E47" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="48" spans="2:5">
       <c r="B48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" t="s">
         <v>14</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>15</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>16</v>
-      </c>
-      <c r="E48" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="49" spans="2:5">
       <c r="B49" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" t="s">
         <v>18</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>19</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>20</v>
-      </c>
-      <c r="E49" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1156,7 +1148,7 @@
   <dimension ref="A1:F31517"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1168,7 +1160,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1">
         <v>0.0005</v>
@@ -1179,7 +1171,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1">
         <v>0.001</v>
@@ -1190,7 +1182,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1">
         <v>0.0015</v>
@@ -1201,7 +1193,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1">
         <v>0.002</v>
@@ -1212,7 +1204,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1">
         <v>0.0025</v>

</xml_diff>